<commit_message>
Done Scripting SCD0291 until SCD0293
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0290 - Admin WEM mengajukan data Non Sales.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0290 - Admin WEM mengajukan data Non Sales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A2E121-A3FF-4F38-8D75-D039304DB463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA87CE9-268D-455C-B7F0-7E4547FE36CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0290" sheetId="2" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </t>
   </si>
   <si>
-    <t>•Pada report Status Tidak Sales berubah</t>
+    <t>•Pada report Status Sales Tidak berubah</t>
   </si>
 </sst>
 </file>
@@ -200,41 +200,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,204 +541,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.42578125" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="4">
         <v>37679</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="15">
+      <c r="L2" s="4">
         <v>54089</v>
       </c>
-      <c r="M2" s="14" t="str">
+      <c r="M2" s="6" t="str">
         <f ca="1">TEXT(TODAY(),"yyyy-mm-dd")</f>
-        <v>2022-08-31</v>
-      </c>
-      <c r="N2" s="14" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="N2" s="6" t="str">
         <f ca="1">TEXT(TODAY()+30,"yyyy-mm-dd")</f>
-        <v>2022-09-30</v>
-      </c>
-      <c r="O2" s="11" t="s">
+        <v>2022-10-01</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="4">
         <v>54089</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="4">
         <v>54089</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>2022</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="2"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="2"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>